<commit_message>
Initial commit: VECM article (Rmd, R scripts, TeX)
</commit_message>
<xml_diff>
--- a/data/mydata.xlsx
+++ b/data/mydata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7dc66aa85898d3af/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{88EC74C0-9A60-4E5C-88F4-126DA568CE4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578E9E0F-5E81-4D96-97FC-2E72988C409F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>profit</t>
+    <t>year</t>
   </si>
   <si>
-    <t>surplusvalue</t>
+    <t>profit</t>
   </si>
   <si>
     <t>occ</t>
   </si>
   <si>
-    <t>year</t>
+    <t>surplusvalue</t>
   </si>
 </sst>
 </file>
@@ -435,19 +435,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>

</xml_diff>